<commit_message>
ahora funciona en todos lados lados lados
</commit_message>
<xml_diff>
--- a/Reporte_Final.xlsx
+++ b/Reporte_Final.xlsx
@@ -528,7 +528,7 @@
         <v>0</v>
       </c>
       <c r="D2">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="E2">
         <v>9</v>
@@ -537,25 +537,25 @@
         <v>0</v>
       </c>
       <c r="G2">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="H2">
         <v>100</v>
       </c>
       <c r="I2">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="J2">
         <v>30</v>
       </c>
       <c r="K2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L2">
         <v>24</v>
       </c>
       <c r="M2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N2">
         <v>4</v>
@@ -588,28 +588,28 @@
         <v>0</v>
       </c>
       <c r="D3">
-        <v>49</v>
+        <v>65</v>
       </c>
       <c r="E3">
-        <v>22</v>
+        <v>26</v>
       </c>
       <c r="F3">
         <v>1</v>
       </c>
       <c r="G3">
-        <v>37</v>
+        <v>52</v>
       </c>
       <c r="H3">
         <v>100</v>
       </c>
       <c r="I3">
-        <v>15</v>
+        <v>27</v>
       </c>
       <c r="J3">
         <v>30</v>
       </c>
       <c r="K3">
-        <v>14</v>
+        <v>24</v>
       </c>
       <c r="L3">
         <v>24</v>
@@ -650,16 +650,16 @@
         <v>0</v>
       </c>
       <c r="D4">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E4">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="F4">
         <v>3</v>
       </c>
       <c r="G4">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="H4">
         <v>100</v>
@@ -710,28 +710,28 @@
         <v>0</v>
       </c>
       <c r="D5">
-        <v>39</v>
+        <v>53</v>
       </c>
       <c r="E5">
-        <v>24</v>
+        <v>35</v>
       </c>
       <c r="F5">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="G5">
-        <v>34</v>
+        <v>45</v>
       </c>
       <c r="H5">
         <v>100</v>
       </c>
       <c r="I5">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="J5">
         <v>30</v>
       </c>
       <c r="K5">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="L5">
         <v>24</v>
@@ -832,34 +832,34 @@
         <v>0</v>
       </c>
       <c r="D7">
-        <v>27</v>
+        <v>35</v>
       </c>
       <c r="E7">
-        <v>18</v>
+        <v>23</v>
       </c>
       <c r="F7">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G7">
-        <v>23</v>
+        <v>30</v>
       </c>
       <c r="H7">
         <v>100</v>
       </c>
       <c r="I7">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="J7">
         <v>30</v>
       </c>
       <c r="K7">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="L7">
         <v>24</v>
       </c>
       <c r="M7">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="N7">
         <v>4</v>
@@ -894,16 +894,16 @@
         <v>0</v>
       </c>
       <c r="D8">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="E8">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="F8">
         <v>0</v>
       </c>
       <c r="G8">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="H8">
         <v>100</v>
@@ -954,28 +954,28 @@
         <v>0</v>
       </c>
       <c r="D9">
-        <v>43</v>
+        <v>52</v>
       </c>
       <c r="E9">
-        <v>33</v>
+        <v>39</v>
       </c>
       <c r="F9">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="G9">
-        <v>36</v>
+        <v>45</v>
       </c>
       <c r="H9">
         <v>100</v>
       </c>
       <c r="I9">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="J9">
         <v>30</v>
       </c>
       <c r="K9">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="L9">
         <v>24</v>
@@ -1016,34 +1016,34 @@
         <v>0</v>
       </c>
       <c r="D10">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="E10">
         <v>26</v>
       </c>
       <c r="F10">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="G10">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="H10">
         <v>100</v>
       </c>
       <c r="I10">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="J10">
         <v>30</v>
       </c>
       <c r="K10">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="L10">
         <v>24</v>
       </c>
       <c r="M10">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="N10">
         <v>4</v>
@@ -1076,34 +1076,34 @@
         <v>0</v>
       </c>
       <c r="D11">
+        <v>12</v>
+      </c>
+      <c r="E11">
+        <v>0</v>
+      </c>
+      <c r="F11">
         <v>5</v>
       </c>
-      <c r="E11">
-        <v>0</v>
-      </c>
-      <c r="F11">
-        <v>3</v>
-      </c>
       <c r="G11">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="H11">
         <v>100</v>
       </c>
       <c r="I11">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="J11">
         <v>30</v>
       </c>
       <c r="K11">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="L11">
         <v>24</v>
       </c>
       <c r="M11">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="N11">
         <v>4</v>

</xml_diff>